<commit_message>
Handling encoding in fread_fwf
</commit_message>
<xml_diff>
--- a/inst/extdata/SchemaSNHS.xlsx
+++ b/inst/extdata/SchemaSNHS.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4994" uniqueCount="4036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4998" uniqueCount="4038">
   <si>
     <t>ACTIVa</t>
   </si>
@@ -12160,6 +12160,12 @@
   </si>
   <si>
     <t>0020</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>()*</t>
   </si>
 </sst>
 </file>
@@ -13276,10 +13282,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.42578125" defaultRowHeight="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14465,6 +14471,29 @@
       </c>
       <c r="G51" s="15" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>4036</v>
+      </c>
+      <c r="B52" s="9">
+        <v>15</v>
+      </c>
+      <c r="C52" s="9">
+        <v>103</v>
+      </c>
+      <c r="D52" s="8">
+        <v>117</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>4037</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>4036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>